<commit_message>
add pandas for data analysis
</commit_message>
<xml_diff>
--- a/checkee.xlsx
+++ b/checkee.xlsx
@@ -429,13 +429,13 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>10599</v>
+        <v>10672</v>
       </c>
       <c r="D2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E2">
-        <v>886</v>
+        <v>896</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -446,13 +446,13 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>1450</v>
+        <v>1455</v>
       </c>
       <c r="D3">
         <v>7</v>
       </c>
       <c r="E3">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -463,7 +463,7 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>7003</v>
+        <v>7030</v>
       </c>
       <c r="D4">
         <v>23</v>
@@ -480,13 +480,13 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>1951</v>
+        <v>1966</v>
       </c>
       <c r="D5">
         <v>13</v>
       </c>
       <c r="E5">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -497,13 +497,13 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>910</v>
+        <v>915</v>
       </c>
       <c r="D6">
         <v>3</v>
       </c>
       <c r="E6">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -514,7 +514,7 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="D7">
         <v>1</v>

</xml_diff>